<commit_message>
more cleanup and table generation
</commit_message>
<xml_diff>
--- a/results/20250305-214416-pol_sci_1/cross_grading_table.xlsx
+++ b/results/20250305-214416-pol_sci_1/cross_grading_table.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Cross Grading" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Cross Grading (Letter Only)" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -27,17 +27,17 @@
     </font>
     <font>
       <name val="Helvetica Neue"/>
-      <b val="1"/>
-      <sz val="5"/>
-    </font>
-    <font>
-      <name val="Helvetica Neue"/>
       <sz val="8"/>
     </font>
     <font>
       <name val="Helvetica Neue"/>
       <b val="1"/>
       <sz val="8"/>
+    </font>
+    <font>
+      <name val="Helvetica Neue"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="7">
@@ -96,38 +96,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -493,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,31 +511,30 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="4.571428571428571" customWidth="1" min="2" max="2"/>
-    <col width="4.571428571428571" customWidth="1" min="3" max="3"/>
-    <col width="4.571428571428571" customWidth="1" min="4" max="4"/>
-    <col width="4.571428571428571" customWidth="1" min="5" max="5"/>
-    <col width="4.571428571428571" customWidth="1" min="6" max="6"/>
-    <col width="4.571428571428571" customWidth="1" min="7" max="7"/>
-    <col width="4.571428571428571" customWidth="1" min="8" max="8"/>
-    <col width="4.571428571428571" customWidth="1" min="9" max="9"/>
-    <col width="4.571428571428571" customWidth="1" min="10" max="10"/>
-    <col width="4.571428571428571" customWidth="1" min="11" max="11"/>
-    <col width="4.571428571428571" customWidth="1" min="12" max="12"/>
-    <col width="4.571428571428571" customWidth="1" min="13" max="13"/>
-    <col width="4.571428571428571" customWidth="1" min="14" max="14"/>
-    <col width="4.571428571428571" customWidth="1" min="15" max="15"/>
-    <col width="4.571428571428571" customWidth="1" min="16" max="16"/>
-    <col width="4.571428571428571" customWidth="1" min="17" max="17"/>
-    <col width="4.571428571428571" customWidth="1" min="18" max="18"/>
-    <col width="4.571428571428571" customWidth="1" min="19" max="19"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="18" max="18"/>
     <col width="12" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Table 1: chatbot cross assessment of each other's responses:</t>
+          <t>Cross-Grading Table: Models Evaluating Each Other's Essays</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
@@ -552,32 +560,32 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Model</t>
+          <t>Model Being Evaluated (Essay Author)</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>o1-mini</t>
+          <t>o1 (Run 1)</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>GPT-4o-mini</t>
+          <t>GPT-4o (Run 1)</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>Claude-3.7-Sonnet</t>
+          <t>Claude 3.7 Sonnet</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>Claude-3-Sonnet</t>
+          <t>Claude 3 Sonnet</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>GPT-4o</t>
+          <t>GPT-4o (Run 2)</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
@@ -587,7 +595,7 @@
       </c>
       <c r="H2" s="3" t="inlineStr">
         <is>
-          <t>DeepSeek-Distill-Qwen-32b</t>
+          <t>DeepSeek 32b</t>
         </is>
       </c>
       <c r="I2" s="3" t="inlineStr">
@@ -597,27 +605,27 @@
       </c>
       <c r="J2" s="3" t="inlineStr">
         <is>
-          <t>grok2-1212</t>
+          <t>Grok 2</t>
         </is>
       </c>
       <c r="K2" s="3" t="inlineStr">
         <is>
-          <t>Perplexity: Llama 3.1 Sonar 8B Online</t>
+          <t>Perplexity 8B</t>
         </is>
       </c>
       <c r="L2" s="3" t="inlineStr">
         <is>
-          <t>Perplexity: Llama 3.1 Sonar 70B</t>
+          <t>Perplexity 70B</t>
         </is>
       </c>
       <c r="M2" s="3" t="inlineStr">
         <is>
-          <t>o1</t>
+          <t>o1 (Run 2)</t>
         </is>
       </c>
       <c r="N2" s="3" t="inlineStr">
         <is>
-          <t>o3-mini-high</t>
+          <t>o3</t>
         </is>
       </c>
       <c r="O2" s="3" t="inlineStr">
@@ -627,17 +635,17 @@
       </c>
       <c r="P2" s="3" t="inlineStr">
         <is>
-          <t>Claude-3-Opus</t>
+          <t>Claude 3 Opus</t>
         </is>
       </c>
       <c r="Q2" s="3" t="inlineStr">
         <is>
-          <t>Claude-3.7-Sonnet-thinking</t>
+          <t>Claude 3.7 Sonnet-thinking</t>
         </is>
       </c>
       <c r="R2" s="3" t="inlineStr">
         <is>
-          <t>DeepSeek-R1-Full</t>
+          <t>DeepSeek R1</t>
         </is>
       </c>
       <c r="S2" s="3" t="inlineStr">
@@ -647,104 +655,104 @@
       </c>
       <c r="T2" s="4" t="inlineStr">
         <is>
-          <t>Raw Numeric Average</t>
+          <t>Overall Score (0-4.25 scale)</t>
         </is>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
       <c r="A3" s="5" t="inlineStr">
         <is>
-          <t>o1-mini</t>
+          <t>o1</t>
         </is>
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="C3" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="D3" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="E3" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="F3" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="G3" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="H3" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="I3" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="J3" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="K3" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="L3" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="M3" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="N3" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="O3" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="P3" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="Q3" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="R3" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="S3" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.63</t>
         </is>
       </c>
       <c r="T3" s="8" t="inlineStr">
@@ -756,97 +764,97 @@
     <row r="4" ht="30" customHeight="1">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>GPT-4o-mini</t>
+          <t>GPT-4o</t>
         </is>
       </c>
       <c r="B4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="C4" s="6" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="D4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="E4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="F4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="G4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="H4" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="I4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="J4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="K4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="L4" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="M4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="N4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="O4" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="P4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="Q4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="R4" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="S4" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.56</t>
         </is>
       </c>
       <c r="T4" s="8" t="inlineStr">
@@ -858,97 +866,97 @@
     <row r="5" ht="30" customHeight="1">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>Claude-3.7-Sonnet</t>
+          <t>Claude 3.7 Sonnet</t>
         </is>
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="D5" s="6" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="E5" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="F5" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="G5" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="H5" s="7" t="inlineStr">
         <is>
-          <t>C+ (2.25)</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="I5" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="J5" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="K5" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="L5" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="M5" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="N5" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="O5" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="P5" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="Q5" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="R5" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="S5" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.44</t>
         </is>
       </c>
       <c r="T5" s="8" t="inlineStr">
@@ -960,97 +968,97 @@
     <row r="6" ht="30" customHeight="1">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>Claude-3-Sonnet</t>
+          <t>Claude 3 Sonnet</t>
         </is>
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="C6" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="D6" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="E6" s="6" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="F6" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="G6" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="H6" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="I6" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="J6" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="K6" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="L6" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="M6" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="N6" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="O6" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="P6" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="Q6" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="R6" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="S6" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.40</t>
         </is>
       </c>
       <c r="T6" s="8" t="inlineStr">
@@ -1067,92 +1075,92 @@
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="C7" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="D7" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="F7" s="6" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="G7" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="H7" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="I7" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="J7" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="K7" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="L7" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="M7" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="N7" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="O7" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="P7" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="Q7" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="R7" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="S7" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.53</t>
         </is>
       </c>
       <c r="T7" s="8" t="inlineStr">
@@ -1169,92 +1177,92 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="D8" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="F8" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="G8" s="6" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="H8" s="7" t="inlineStr">
         <is>
-          <t>C+ (2.25)</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="I8" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="J8" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="K8" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="L8" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="M8" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="N8" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="O8" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="P8" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="Q8" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="R8" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="S8" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.47</t>
         </is>
       </c>
       <c r="T8" s="8" t="inlineStr">
@@ -1266,97 +1274,97 @@
     <row r="9" ht="30" customHeight="1">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t>DeepSeek-Distill-Qwen-32b</t>
+          <t>DeepSeek 32b</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="C9" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="D9" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="E9" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="F9" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="G9" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="H9" s="6" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="I9" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="K9" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="L9" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="M9" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="N9" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="O9" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="P9" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="Q9" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="R9" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="S9" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>2.82</t>
         </is>
       </c>
       <c r="T9" s="8" t="inlineStr">
@@ -1373,92 +1381,92 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="D10" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="E10" s="7" t="inlineStr">
         <is>
-          <t>B- (2.75)</t>
+          <t>2.75</t>
         </is>
       </c>
       <c r="F10" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="G10" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="H10" s="7" t="inlineStr">
         <is>
-          <t>C+ (2.25)</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="I10" s="6" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="J10" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="K10" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="L10" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="M10" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="N10" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="O10" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="P10" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="Q10" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="R10" s="7" t="inlineStr">
         <is>
-          <t>B- (2.75)</t>
+          <t>2.75</t>
         </is>
       </c>
       <c r="S10" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.47</t>
         </is>
       </c>
       <c r="T10" s="8" t="inlineStr">
@@ -1470,97 +1478,97 @@
     <row r="11" ht="30" customHeight="1">
       <c r="A11" s="5" t="inlineStr">
         <is>
-          <t>grok2-1212</t>
+          <t>Grok 2</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="C11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="D11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="F11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="G11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="H11" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="I11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="J11" s="6" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="K11" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="L11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="M11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="N11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="O11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="P11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="Q11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="R11" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="S11" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.56</t>
         </is>
       </c>
       <c r="T11" s="8" t="inlineStr">
@@ -1572,97 +1580,97 @@
     <row r="12" ht="30" customHeight="1">
       <c r="A12" s="5" t="inlineStr">
         <is>
-          <t>Perplexity: Llama 3.1 Sonar 8B Online</t>
+          <t>Perplexity 8B</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="C12" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="D12" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="E12" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="F12" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="G12" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="H12" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="I12" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="J12" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="K12" s="6" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="L12" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="M12" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="N12" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="O12" s="7" t="inlineStr">
         <is>
-          <t>C (2.00)</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="P12" s="7" t="inlineStr">
         <is>
-          <t>C (2.00)</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="Q12" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="R12" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="S12" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.43</t>
         </is>
       </c>
       <c r="T12" s="8" t="inlineStr">
@@ -1674,97 +1682,97 @@
     <row r="13" ht="30" customHeight="1">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t>Perplexity: Llama 3.1 Sonar 70B</t>
+          <t>Perplexity 70B</t>
         </is>
       </c>
       <c r="B13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="C13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="D13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="E13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="F13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="G13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="H13" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="I13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="J13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="K13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="L13" s="6" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="M13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="N13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="O13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="P13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="Q13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="R13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="S13" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.54</t>
         </is>
       </c>
       <c r="T13" s="8" t="inlineStr">
@@ -1781,92 +1789,92 @@
       </c>
       <c r="B14" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="C14" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="D14" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="E14" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="F14" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="G14" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="H14" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="I14" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="J14" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="K14" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="L14" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="M14" s="6" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="N14" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="O14" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="P14" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="Q14" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="R14" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="S14" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.60</t>
         </is>
       </c>
       <c r="T14" s="8" t="inlineStr">
@@ -1878,97 +1886,97 @@
     <row r="15" ht="30" customHeight="1">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>o3-mini-high</t>
+          <t>o3</t>
         </is>
       </c>
       <c r="B15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="C15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="D15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="E15" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="F15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="G15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="H15" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="I15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="J15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="K15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="L15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="M15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="N15" s="6" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="O15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="P15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="Q15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="R15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="S15" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.60</t>
         </is>
       </c>
       <c r="T15" s="8" t="inlineStr">
@@ -1985,92 +1993,92 @@
       </c>
       <c r="B16" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="C16" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="D16" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="E16" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="F16" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="G16" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="H16" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="I16" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="J16" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="K16" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="L16" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="M16" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="N16" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="O16" s="6" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="P16" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="Q16" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="R16" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="S16" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.62</t>
         </is>
       </c>
       <c r="T16" s="8" t="inlineStr">
@@ -2082,97 +2090,97 @@
     <row r="17" ht="30" customHeight="1">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>Claude-3-Opus</t>
+          <t>Claude 3 Opus</t>
         </is>
       </c>
       <c r="B17" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="C17" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="D17" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="E17" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="F17" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="G17" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="H17" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="I17" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="J17" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="K17" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="L17" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="M17" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="N17" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="O17" s="7" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="P17" s="6" t="inlineStr">
         <is>
-          <t>A (4.00)</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="Q17" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="R17" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="S17" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.56</t>
         </is>
       </c>
       <c r="T17" s="8" t="inlineStr">
@@ -2184,97 +2192,97 @@
     <row r="18" ht="30" customHeight="1">
       <c r="A18" s="5" t="inlineStr">
         <is>
-          <t>Claude-3.7-Sonnet-thinking</t>
+          <t>Claude 3.7 Sonnet-thinking</t>
         </is>
       </c>
       <c r="B18" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="C18" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="D18" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="E18" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="F18" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="G18" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="H18" s="7" t="inlineStr">
         <is>
-          <t>C+ (2.25)</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="I18" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="J18" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="K18" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="L18" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="M18" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="N18" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="O18" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="P18" s="7" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="Q18" s="6" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="R18" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="S18" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.49</t>
         </is>
       </c>
       <c r="T18" s="8" t="inlineStr">
@@ -2286,97 +2294,97 @@
     <row r="19" ht="30" customHeight="1">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>DeepSeek-R1-Full</t>
+          <t>DeepSeek R1</t>
         </is>
       </c>
       <c r="B19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="C19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="D19" s="7" t="inlineStr">
         <is>
-          <t>C (2.00)</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="E19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="F19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="G19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="H19" s="7" t="inlineStr">
         <is>
-          <t>C (2.00)</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="I19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="J19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="K19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="L19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="M19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="N19" s="7" t="inlineStr">
         <is>
-          <t>C (2.00)</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="O19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="P19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="Q19" s="7" t="inlineStr">
         <is>
-          <t>A- (3.75)</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="R19" s="6" t="inlineStr">
         <is>
-          <t>B+ (3.25)</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="S19" s="7" t="inlineStr">
         <is>
-          <t>B (3.00)</t>
+          <t>3.47</t>
         </is>
       </c>
       <c r="T19" s="8" t="inlineStr">
@@ -2388,7 +2396,7 @@
     <row r="20">
       <c r="A20" s="9" t="inlineStr">
         <is>
-          <t>Grading Bias</t>
+          <t>Grading Bias (Lenient/Strict Tendencies)</t>
         </is>
       </c>
       <c r="B20" s="10" t="inlineStr">
@@ -2488,119 +2496,214 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="inlineStr">
-        <is>
-          <t>Column Medians</t>
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Median Grade Given by Model</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>A-
-(Very Good)</t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>A-
-(Very Good)</t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>A-
-(Very Good)</t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>B+
-(Good)</t>
+          <t>87.00</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>A-
-(Very Good)</t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="G21" s="3" t="inlineStr">
         <is>
-          <t>B+
-(Good)</t>
+          <t>87.00</t>
         </is>
       </c>
       <c r="H21" s="3" t="inlineStr">
         <is>
-          <t>B
-(Good)</t>
+          <t>83.00</t>
         </is>
       </c>
       <c r="I21" s="3" t="inlineStr">
         <is>
-          <t>B+
-(Good)</t>
+          <t>87.00</t>
         </is>
       </c>
       <c r="J21" s="3" t="inlineStr">
         <is>
-          <t>A-
-(Very Good)</t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K21" s="3" t="inlineStr">
         <is>
-          <t>B+
-(Good)</t>
+          <t>87.00</t>
         </is>
       </c>
       <c r="L21" s="3" t="inlineStr">
         <is>
-          <t>A-
-(Very Good)</t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="M21" s="3" t="inlineStr">
         <is>
-          <t>A-
-(Very Good)</t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="N21" s="3" t="inlineStr">
         <is>
-          <t>A-
-(Very Good)</t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="O21" s="3" t="inlineStr">
         <is>
-          <t>A-
-(Very Good)</t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="P21" s="3" t="inlineStr">
         <is>
-          <t>A-
-(Very Good)</t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="Q21" s="3" t="inlineStr">
         <is>
-          <t>A-
-(Very Good)</t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="R21" s="3" t="inlineStr">
         <is>
-          <t>B+
-(Good)</t>
-        </is>
-      </c>
-      <c r="S21" s="12" t="inlineStr"/>
-      <c r="T21" s="12" t="inlineStr"/>
+          <t>87.00</t>
+        </is>
+      </c>
+      <c r="S21" s="13" t="inlineStr"/>
+      <c r="T21" s="13" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="14" t="inlineStr">
+        <is>
+          <t>Table Legend:</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="15" t="inlineStr">
+        <is>
+          <t>- Rows: Each row represents a model being evaluated (essay author)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="15" t="inlineStr">
+        <is>
+          <t>- Columns: Each column shows the score given by a particular grading model</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="15" t="inlineStr">
+        <is>
+          <t>- Self-assessments (where a model grades its own essay) are highlighted in lavender</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="15" t="inlineStr">
+        <is>
+          <t>- Overall Score column shows the numerical average of all grades on a 0-4.25 scale</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="14" t="inlineStr">
+        <is>
+          <t>Model Name Reference:</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="15" t="inlineStr">
+        <is>
+          <t>Claude 3.7 Sonnet = Claude-3.7-Sonnet</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="15" t="inlineStr">
+        <is>
+          <t>Claude 3 Sonnet = Claude-3-Sonnet</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="15" t="inlineStr">
+        <is>
+          <t>DeepSeek 32b = DeepSeek-Distill-Qwen-32b</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="15" t="inlineStr">
+        <is>
+          <t>Grok 2 = grok2-1212</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="15" t="inlineStr">
+        <is>
+          <t>Perplexity 8B = Perplexity: Llama 3.1 Sonar 8B Online</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="15" t="inlineStr">
+        <is>
+          <t>Perplexity 70B = Perplexity: Llama 3.1 Sonar 70B</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="15" t="inlineStr">
+        <is>
+          <t>o3 = o3-mini-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="15" t="inlineStr">
+        <is>
+          <t>Claude 3 Opus = Claude-3-Opus</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="15" t="inlineStr">
+        <is>
+          <t>Claude 3.7 Sonnet-thinking = Claude-3.7-Sonnet-thinking</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="15" t="inlineStr">
+        <is>
+          <t>DeepSeek R1 = DeepSeek-R1-Full</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A1:T1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>